<commit_message>
Add : ExitGame message
</commit_message>
<xml_diff>
--- a/Assets/UIMessages.xlsx
+++ b/Assets/UIMessages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\visualstudio workstation\TheMoneyIsAlwaysRight\TheMoneyIsAlwaysRight\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08600B7C-4911-4192-B258-94A1E117A876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E9AF8B-B60E-4B6E-87D3-778113372712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EBB1A9E2-7A33-4440-BC32-B1894732EB92}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>선택지 번호를 입력해주세요</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>#EOS2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#SOS3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOS3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임을 종료합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -454,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA67553B-7E4F-4E0A-96DE-0846ED4D695A}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -493,6 +505,21 @@
         <v>4</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>